<commit_message>
Tester A did it!
</commit_message>
<xml_diff>
--- a/TestBook1.xlsx
+++ b/TestBook1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>This is my test suite</t>
   </si>
@@ -125,14 +125,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +416,7 @@
   <dimension ref="C3:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,84 +425,90 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="2" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="2" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="K7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="2" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="2" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="2"/>
+      <c r="K8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="2" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="2" t="s">
+      <c r="H9" s="4"/>
+      <c r="I9" s="2"/>
+      <c r="K9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Tester B did it!
</commit_message>
<xml_diff>
--- a/TestBook1.xlsx
+++ b/TestBook1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>This is my test suite</t>
   </si>
@@ -125,14 +125,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +416,7 @@
   <dimension ref="C3:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,84 +425,90 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="2" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="2" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="2" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="2" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="2" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="2" t="s">
+      <c r="H9" s="4"/>
+      <c r="I9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>